<commit_message>
add lc16-ecommerce + lc18-vanilla-js-contentFul
</commit_message>
<xml_diff>
--- a/code.xlsx
+++ b/code.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Symfony\Code\MyWEB-Codev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943A8AB0-D9C6-41F1-8FD3-169CB878E3D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3FFE9E-E7FA-4C76-9F6E-DF089189EE9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="32">
   <si>
     <t>Folders</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>codev-yt-ecommerce-2</t>
+  </si>
+  <si>
+    <t>codev-lc16-ecommerce-website</t>
+  </si>
+  <si>
+    <t>codev-lc18-vanilla-js</t>
   </si>
 </sst>
 </file>
@@ -495,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I17"/>
+      <selection activeCell="I7" sqref="I7:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -820,7 +826,7 @@
         <v>10</v>
       </c>
       <c r="G6" s="3" t="str">
-        <f t="shared" ref="G6:G17" si="3">_xlfn.CONCAT($B6,$A6,$C6,$A6,$D6)</f>
+        <f t="shared" ref="G6:G19" si="3">_xlfn.CONCAT($B6,$A6,$C6,$A6,$D6)</f>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
         &lt;a href="src/codev-lc10-realestate/index.html" target="_blank"&gt;codev-lc10-realestate&lt;/a&gt;
@@ -830,7 +836,7 @@
             title="</v>
       </c>
       <c r="H6" s="3" t="str">
-        <f t="shared" ref="H6:H17" si="4">_xlfn.CONCAT($A6,$E6,$A6,$F6)</f>
+        <f t="shared" ref="H6:H19" si="4">_xlfn.CONCAT($A6,$E6,$A6,$F6)</f>
         <v xml:space="preserve">codev-lc10-realestate"
             width="460"
             height="315"
@@ -844,7 +850,7 @@
       </v>
       </c>
       <c r="I6" s="7" t="str">
-        <f t="shared" ref="I6:I17" si="5">_xlfn.CONCAT($G6,$H6)</f>
+        <f t="shared" ref="I6:I19" si="5">_xlfn.CONCAT($G6,$H6)</f>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
         &lt;a href="src/codev-lc10-realestate/index.html" target="_blank"&gt;codev-lc10-realestate&lt;/a&gt;
@@ -866,7 +872,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -887,7 +893,7 @@
         <f t="shared" si="3"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-phone_website/index.html" target="_blank"&gt;codev-phone_website&lt;/a&gt;
+        &lt;a href="src/codev-lc16-ecommerce-website/index.html" target="_blank"&gt;codev-lc16-ecommerce-website&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -895,10 +901,10 @@
       </c>
       <c r="H7" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">codev-phone_website"
-            width="460"
-            height="315"
-            src="src/codev-phone_website/index.html"
+        <v xml:space="preserve">codev-lc16-ecommerce-website"
+            width="460"
+            height="315"
+            src="src/codev-lc16-ecommerce-website/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -911,14 +917,14 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-phone_website/index.html" target="_blank"&gt;codev-phone_website&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="codev-phone_website"
-            width="460"
-            height="315"
-            src="src/codev-phone_website/index.html"
+        &lt;a href="src/codev-lc16-ecommerce-website/index.html" target="_blank"&gt;codev-lc16-ecommerce-website&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="codev-lc16-ecommerce-website"
+            width="460"
+            height="315"
+            src="src/codev-lc16-ecommerce-website/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -930,7 +936,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
@@ -951,7 +957,7 @@
         <f t="shared" si="3"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-portfolio-6/index.html" target="_blank"&gt;codev-portfolio-6&lt;/a&gt;
+        &lt;a href="src/codev-lc18-vanilla-js/index.html" target="_blank"&gt;codev-lc18-vanilla-js&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -959,10 +965,10 @@
       </c>
       <c r="H8" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">codev-portfolio-6"
-            width="460"
-            height="315"
-            src="src/codev-portfolio-6/index.html"
+        <v xml:space="preserve">codev-lc18-vanilla-js"
+            width="460"
+            height="315"
+            src="src/codev-lc18-vanilla-js/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -975,14 +981,14 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-portfolio-6/index.html" target="_blank"&gt;codev-portfolio-6&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="codev-portfolio-6"
-            width="460"
-            height="315"
-            src="src/codev-portfolio-6/index.html"
+        &lt;a href="src/codev-lc18-vanilla-js/index.html" target="_blank"&gt;codev-lc18-vanilla-js&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="codev-lc18-vanilla-js"
+            width="460"
+            height="315"
+            src="src/codev-lc18-vanilla-js/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -994,7 +1000,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
@@ -1015,7 +1021,7 @@
         <f t="shared" si="3"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-portfolio-8/index.html" target="_blank"&gt;codev-portfolio-8&lt;/a&gt;
+        &lt;a href="src/codev-phone_website/index.html" target="_blank"&gt;codev-phone_website&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -1023,10 +1029,10 @@
       </c>
       <c r="H9" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">codev-portfolio-8"
-            width="460"
-            height="315"
-            src="src/codev-portfolio-8/index.html"
+        <v xml:space="preserve">codev-phone_website"
+            width="460"
+            height="315"
+            src="src/codev-phone_website/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1039,14 +1045,14 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-portfolio-8/index.html" target="_blank"&gt;codev-portfolio-8&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="codev-portfolio-8"
-            width="460"
-            height="315"
-            src="src/codev-portfolio-8/index.html"
+        &lt;a href="src/codev-phone_website/index.html" target="_blank"&gt;codev-phone_website&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="codev-phone_website"
+            width="460"
+            height="315"
+            src="src/codev-phone_website/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1058,7 +1064,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
@@ -1079,7 +1085,7 @@
         <f t="shared" si="3"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-portfolio-test/index.html" target="_blank"&gt;codev-portfolio-test&lt;/a&gt;
+        &lt;a href="src/codev-portfolio-6/index.html" target="_blank"&gt;codev-portfolio-6&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -1087,10 +1093,10 @@
       </c>
       <c r="H10" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">codev-portfolio-test"
-            width="460"
-            height="315"
-            src="src/codev-portfolio-test/index.html"
+        <v xml:space="preserve">codev-portfolio-6"
+            width="460"
+            height="315"
+            src="src/codev-portfolio-6/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1103,14 +1109,14 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-portfolio-test/index.html" target="_blank"&gt;codev-portfolio-test&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="codev-portfolio-test"
-            width="460"
-            height="315"
-            src="src/codev-portfolio-test/index.html"
+        &lt;a href="src/codev-portfolio-6/index.html" target="_blank"&gt;codev-portfolio-6&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="codev-portfolio-6"
+            width="460"
+            height="315"
+            src="src/codev-portfolio-6/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1122,7 +1128,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -1143,7 +1149,7 @@
         <f t="shared" si="3"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-portfolio-website/index.html" target="_blank"&gt;codev-portfolio-website&lt;/a&gt;
+        &lt;a href="src/codev-portfolio-8/index.html" target="_blank"&gt;codev-portfolio-8&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -1151,10 +1157,10 @@
       </c>
       <c r="H11" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">codev-portfolio-website"
-            width="460"
-            height="315"
-            src="src/codev-portfolio-website/index.html"
+        <v xml:space="preserve">codev-portfolio-8"
+            width="460"
+            height="315"
+            src="src/codev-portfolio-8/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1167,14 +1173,14 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-portfolio-website/index.html" target="_blank"&gt;codev-portfolio-website&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="codev-portfolio-website"
-            width="460"
-            height="315"
-            src="src/codev-portfolio-website/index.html"
+        &lt;a href="src/codev-portfolio-8/index.html" target="_blank"&gt;codev-portfolio-8&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="codev-portfolio-8"
+            width="460"
+            height="315"
+            src="src/codev-portfolio-8/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1186,7 +1192,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -1207,7 +1213,7 @@
         <f t="shared" si="3"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-portfolio2/index.html" target="_blank"&gt;codev-portfolio2&lt;/a&gt;
+        &lt;a href="src/codev-portfolio-test/index.html" target="_blank"&gt;codev-portfolio-test&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -1215,10 +1221,10 @@
       </c>
       <c r="H12" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">codev-portfolio2"
-            width="460"
-            height="315"
-            src="src/codev-portfolio2/index.html"
+        <v xml:space="preserve">codev-portfolio-test"
+            width="460"
+            height="315"
+            src="src/codev-portfolio-test/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1231,14 +1237,14 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-portfolio2/index.html" target="_blank"&gt;codev-portfolio2&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="codev-portfolio2"
-            width="460"
-            height="315"
-            src="src/codev-portfolio2/index.html"
+        &lt;a href="src/codev-portfolio-test/index.html" target="_blank"&gt;codev-portfolio-test&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="codev-portfolio-test"
+            width="460"
+            height="315"
+            src="src/codev-portfolio-test/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1250,7 +1256,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
@@ -1271,7 +1277,7 @@
         <f t="shared" si="3"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-portfolio3/index.html" target="_blank"&gt;codev-portfolio3&lt;/a&gt;
+        &lt;a href="src/codev-portfolio-website/index.html" target="_blank"&gt;codev-portfolio-website&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -1279,10 +1285,10 @@
       </c>
       <c r="H13" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">codev-portfolio3"
-            width="460"
-            height="315"
-            src="src/codev-portfolio3/index.html"
+        <v xml:space="preserve">codev-portfolio-website"
+            width="460"
+            height="315"
+            src="src/codev-portfolio-website/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1295,14 +1301,14 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-portfolio3/index.html" target="_blank"&gt;codev-portfolio3&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="codev-portfolio3"
-            width="460"
-            height="315"
-            src="src/codev-portfolio3/index.html"
+        &lt;a href="src/codev-portfolio-website/index.html" target="_blank"&gt;codev-portfolio-website&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="codev-portfolio-website"
+            width="460"
+            height="315"
+            src="src/codev-portfolio-website/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1314,7 +1320,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
@@ -1335,7 +1341,7 @@
         <f t="shared" si="3"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-portfolio_02/index.html" target="_blank"&gt;codev-portfolio_02&lt;/a&gt;
+        &lt;a href="src/codev-portfolio2/index.html" target="_blank"&gt;codev-portfolio2&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -1343,10 +1349,10 @@
       </c>
       <c r="H14" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">codev-portfolio_02"
-            width="460"
-            height="315"
-            src="src/codev-portfolio_02/index.html"
+        <v xml:space="preserve">codev-portfolio2"
+            width="460"
+            height="315"
+            src="src/codev-portfolio2/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1359,14 +1365,14 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-portfolio_02/index.html" target="_blank"&gt;codev-portfolio_02&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="codev-portfolio_02"
-            width="460"
-            height="315"
-            src="src/codev-portfolio_02/index.html"
+        &lt;a href="src/codev-portfolio2/index.html" target="_blank"&gt;codev-portfolio2&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="codev-portfolio2"
+            width="460"
+            height="315"
+            src="src/codev-portfolio2/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1378,7 +1384,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
@@ -1399,7 +1405,7 @@
         <f t="shared" si="3"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-travel-website/index.html" target="_blank"&gt;codev-travel-website&lt;/a&gt;
+        &lt;a href="src/codev-portfolio3/index.html" target="_blank"&gt;codev-portfolio3&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -1407,10 +1413,10 @@
       </c>
       <c r="H15" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">codev-travel-website"
-            width="460"
-            height="315"
-            src="src/codev-travel-website/index.html"
+        <v xml:space="preserve">codev-portfolio3"
+            width="460"
+            height="315"
+            src="src/codev-portfolio3/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1423,14 +1429,14 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-travel-website/index.html" target="_blank"&gt;codev-travel-website&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="codev-travel-website"
-            width="460"
-            height="315"
-            src="src/codev-travel-website/index.html"
+        &lt;a href="src/codev-portfolio3/index.html" target="_blank"&gt;codev-portfolio3&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="codev-portfolio3"
+            width="460"
+            height="315"
+            src="src/codev-portfolio3/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1442,7 +1448,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>3</v>
@@ -1463,7 +1469,7 @@
         <f t="shared" si="3"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-video-background/index.html" target="_blank"&gt;codev-video-background&lt;/a&gt;
+        &lt;a href="src/codev-portfolio_02/index.html" target="_blank"&gt;codev-portfolio_02&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -1471,10 +1477,10 @@
       </c>
       <c r="H16" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">codev-video-background"
-            width="460"
-            height="315"
-            src="src/codev-video-background/index.html"
+        <v xml:space="preserve">codev-portfolio_02"
+            width="460"
+            height="315"
+            src="src/codev-portfolio_02/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1487,14 +1493,14 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-video-background/index.html" target="_blank"&gt;codev-video-background&lt;/a&gt;
-        &lt;hr class="rounded" /&gt;
-        &lt;div&gt;
-          &lt;iframe
-            title="codev-video-background"
-            width="460"
-            height="315"
-            src="src/codev-video-background/index.html"
+        &lt;a href="src/codev-portfolio_02/index.html" target="_blank"&gt;codev-portfolio_02&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="codev-portfolio_02"
+            width="460"
+            height="315"
+            src="src/codev-portfolio_02/index.html"
             frameborder="0"
             allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
             allowfullscreen
@@ -1506,7 +1512,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>3</v>
@@ -1527,7 +1533,7 @@
         <f t="shared" si="3"/>
         <v>&lt;section&gt;
         &lt;hr class="rounded" /&gt;
-        &lt;a href="src/codev-yt-ecommerce-2/index.html" target="_blank"&gt;codev-yt-ecommerce-2&lt;/a&gt;
+        &lt;a href="src/codev-travel-website/index.html" target="_blank"&gt;codev-travel-website&lt;/a&gt;
         &lt;hr class="rounded" /&gt;
         &lt;div&gt;
           &lt;iframe
@@ -1535,6 +1541,134 @@
       </c>
       <c r="H17" s="3" t="str">
         <f t="shared" si="4"/>
+        <v xml:space="preserve">codev-travel-website"
+            width="460"
+            height="315"
+            src="src/codev-travel-website/index.html"
+            frameborder="0"
+            allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
+            allowfullscreen
+          &gt;&lt;/iframe&gt;
+        &lt;/div&gt;
+      &lt;/section&gt;
+      </v>
+      </c>
+      <c r="I17" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">&lt;section&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;a href="src/codev-travel-website/index.html" target="_blank"&gt;codev-travel-website&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="codev-travel-website"
+            width="460"
+            height="315"
+            src="src/codev-travel-website/index.html"
+            frameborder="0"
+            allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
+            allowfullscreen
+          &gt;&lt;/iframe&gt;
+        &lt;/div&gt;
+      &lt;/section&gt;
+      </v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;section&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;a href="src/codev-video-background/index.html" target="_blank"&gt;codev-video-background&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="</v>
+      </c>
+      <c r="H18" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">codev-video-background"
+            width="460"
+            height="315"
+            src="src/codev-video-background/index.html"
+            frameborder="0"
+            allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
+            allowfullscreen
+          &gt;&lt;/iframe&gt;
+        &lt;/div&gt;
+      &lt;/section&gt;
+      </v>
+      </c>
+      <c r="I18" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">&lt;section&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;a href="src/codev-video-background/index.html" target="_blank"&gt;codev-video-background&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="codev-video-background"
+            width="460"
+            height="315"
+            src="src/codev-video-background/index.html"
+            frameborder="0"
+            allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture"
+            allowfullscreen
+          &gt;&lt;/iframe&gt;
+        &lt;/div&gt;
+      &lt;/section&gt;
+      </v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;section&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;a href="src/codev-yt-ecommerce-2/index.html" target="_blank"&gt;codev-yt-ecommerce-2&lt;/a&gt;
+        &lt;hr class="rounded" /&gt;
+        &lt;div&gt;
+          &lt;iframe
+            title="</v>
+      </c>
+      <c r="H19" s="3" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">codev-yt-ecommerce-2"
             width="460"
             height="315"
@@ -1547,7 +1681,7 @@
       &lt;/section&gt;
       </v>
       </c>
-      <c r="I17" s="7" t="str">
+      <c r="I19" s="7" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">&lt;section&gt;
         &lt;hr class="rounded" /&gt;

</xml_diff>